<commit_message>
Generate Report for employee
</commit_message>
<xml_diff>
--- a/server/src/main/resources/template/excel/REPORT_WORKER_TEMPLATE.xlsx
+++ b/server/src/main/resources/template/excel/REPORT_WORKER_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Ewid roczna" sheetId="1" r:id="rId4"/>
+    <sheet name="REPORT_RECORD" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -16,7 +16,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ROCZNA KARTA EWIDENCJI CZASU PRACY za rok 2020</t>
+    <t>ROCZNA KARTA EWIDENCJI CZASU PRACY za rok #YEAR</t>
   </si>
   <si>
     <t>Pieczęć jednostki organizacyjnej</t>
@@ -178,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -252,12 +252,6 @@
     <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -267,16 +261,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial CE"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="13"/>
-      <name val="Arial CE"/>
-    </font>
-    <font>
       <sz val="4"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -284,11 +268,6 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Times New Roman CE"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="12"/>
       <name val="Times New Roman CE"/>
     </font>
     <font>
@@ -1045,7 +1024,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1211,10 +1190,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1241,22 +1217,13 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1271,21 +1238,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1298,28 +1256,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1337,13 +1289,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="47" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1374,9 +1326,6 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff000080"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff008000"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2446,7 +2395,7 @@
   <cols>
     <col min="1" max="1" width="7.8125" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.8125" style="1" customWidth="1"/>
-    <col min="3" max="49" width="3.60156" style="1" customWidth="1"/>
+    <col min="3" max="49" width="5.21094" style="1" customWidth="1"/>
     <col min="50" max="16384" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2906,1699 +2855,1699 @@
       <c r="C9" s="54">
         <v>1</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="54">
         <v>2</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="54">
         <v>3</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="54">
         <v>4</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="54">
         <v>5</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="54">
         <v>6</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="54">
         <v>7</v>
       </c>
-      <c r="J9" s="55">
+      <c r="J9" s="54">
         <v>8</v>
       </c>
-      <c r="K9" s="55">
+      <c r="K9" s="54">
         <v>9</v>
       </c>
-      <c r="L9" s="55">
+      <c r="L9" s="54">
         <v>10</v>
       </c>
-      <c r="M9" s="55">
+      <c r="M9" s="54">
         <v>11</v>
       </c>
-      <c r="N9" s="55">
+      <c r="N9" s="54">
         <v>12</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="54">
         <v>13</v>
       </c>
-      <c r="P9" s="55">
+      <c r="P9" s="54">
         <v>14</v>
       </c>
-      <c r="Q9" s="55">
+      <c r="Q9" s="54">
         <v>15</v>
       </c>
-      <c r="R9" s="55">
+      <c r="R9" s="54">
         <v>16</v>
       </c>
-      <c r="S9" s="55">
+      <c r="S9" s="54">
         <v>17</v>
       </c>
-      <c r="T9" s="55">
+      <c r="T9" s="54">
         <v>18</v>
       </c>
-      <c r="U9" s="55">
+      <c r="U9" s="54">
         <v>19</v>
       </c>
-      <c r="V9" s="55">
+      <c r="V9" s="54">
         <v>20</v>
       </c>
-      <c r="W9" s="55">
+      <c r="W9" s="54">
         <v>21</v>
       </c>
-      <c r="X9" s="55">
+      <c r="X9" s="54">
         <v>22</v>
       </c>
-      <c r="Y9" s="55">
+      <c r="Y9" s="54">
         <v>23</v>
       </c>
-      <c r="Z9" s="55">
+      <c r="Z9" s="54">
         <v>24</v>
       </c>
-      <c r="AA9" s="55">
+      <c r="AA9" s="54">
         <v>25</v>
       </c>
-      <c r="AB9" s="55">
+      <c r="AB9" s="54">
         <v>26</v>
       </c>
-      <c r="AC9" s="55">
+      <c r="AC9" s="54">
         <v>27</v>
       </c>
-      <c r="AD9" s="55">
+      <c r="AD9" s="54">
         <v>28</v>
       </c>
-      <c r="AE9" s="55">
+      <c r="AE9" s="54">
         <v>29</v>
       </c>
-      <c r="AF9" s="55">
+      <c r="AF9" s="54">
         <v>30</v>
       </c>
-      <c r="AG9" s="56">
+      <c r="AG9" s="55">
         <v>31</v>
       </c>
-      <c r="AH9" t="s" s="57">
+      <c r="AH9" t="s" s="56">
         <v>20</v>
       </c>
-      <c r="AI9" t="s" s="58">
+      <c r="AI9" t="s" s="57">
         <v>21</v>
       </c>
-      <c r="AJ9" t="s" s="58">
+      <c r="AJ9" t="s" s="57">
         <v>22</v>
       </c>
-      <c r="AK9" t="s" s="58">
+      <c r="AK9" t="s" s="57">
         <v>23</v>
       </c>
-      <c r="AL9" t="s" s="59">
+      <c r="AL9" t="s" s="58">
         <v>24</v>
       </c>
-      <c r="AM9" s="60"/>
-      <c r="AN9" s="61"/>
-      <c r="AO9" s="61"/>
-      <c r="AP9" s="62"/>
-      <c r="AQ9" s="60"/>
-      <c r="AR9" s="63"/>
-      <c r="AS9" s="62"/>
-      <c r="AT9" s="60"/>
-      <c r="AU9" s="61"/>
-      <c r="AV9" s="61"/>
-      <c r="AW9" s="62"/>
+      <c r="AM9" s="59"/>
+      <c r="AN9" s="60"/>
+      <c r="AO9" s="60"/>
+      <c r="AP9" s="61"/>
+      <c r="AQ9" s="59"/>
+      <c r="AR9" s="62"/>
+      <c r="AS9" s="61"/>
+      <c r="AT9" s="59"/>
+      <c r="AU9" s="60"/>
+      <c r="AV9" s="60"/>
+      <c r="AW9" s="61"/>
     </row>
     <row r="10" ht="17.1" customHeight="1">
-      <c r="A10" t="s" s="64">
+      <c r="A10" t="s" s="63">
         <v>25</v>
       </c>
-      <c r="B10" t="s" s="65">
+      <c r="B10" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="68"/>
-      <c r="U10" s="66"/>
-      <c r="V10" s="66"/>
-      <c r="W10" s="66"/>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="66"/>
-      <c r="AC10" s="66"/>
-      <c r="AD10" t="s" s="70">
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="65"/>
+      <c r="X10" s="65"/>
+      <c r="Y10" s="65"/>
+      <c r="Z10" s="65"/>
+      <c r="AA10" s="65"/>
+      <c r="AB10" s="65"/>
+      <c r="AC10" s="65"/>
+      <c r="AD10" t="s" s="67">
         <v>0</v>
       </c>
-      <c r="AE10" t="s" s="71">
+      <c r="AE10" t="s" s="67">
         <v>0</v>
       </c>
-      <c r="AF10" t="s" s="71">
+      <c r="AF10" t="s" s="67">
         <v>0</v>
       </c>
-      <c r="AG10" t="s" s="71">
+      <c r="AG10" t="s" s="67">
         <v>0</v>
       </c>
-      <c r="AH10" s="72"/>
-      <c r="AI10" s="72"/>
-      <c r="AJ10" s="72"/>
-      <c r="AK10" s="72"/>
-      <c r="AL10" s="72"/>
-      <c r="AM10" t="s" s="73">
+      <c r="AH10" s="68"/>
+      <c r="AI10" s="68"/>
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="68"/>
+      <c r="AL10" s="68"/>
+      <c r="AM10" t="s" s="69">
         <v>0</v>
       </c>
-      <c r="AN10" s="72"/>
-      <c r="AO10" s="72"/>
-      <c r="AP10" s="72"/>
-      <c r="AQ10" s="72"/>
-      <c r="AR10" s="72"/>
-      <c r="AS10" s="72"/>
-      <c r="AT10" s="72"/>
-      <c r="AU10" s="72"/>
-      <c r="AV10" s="72"/>
-      <c r="AW10" s="72"/>
+      <c r="AN10" s="68"/>
+      <c r="AO10" s="68"/>
+      <c r="AP10" s="68"/>
+      <c r="AQ10" s="68"/>
+      <c r="AR10" s="68"/>
+      <c r="AS10" s="68"/>
+      <c r="AT10" s="68"/>
+      <c r="AU10" s="68"/>
+      <c r="AV10" s="68"/>
+      <c r="AW10" s="68"/>
     </row>
     <row r="11" ht="17.1" customHeight="1">
-      <c r="A11" s="74"/>
-      <c r="B11" t="s" s="75">
+      <c r="A11" s="70"/>
+      <c r="B11" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="77"/>
-      <c r="R11" s="77"/>
-      <c r="S11" s="77"/>
-      <c r="T11" s="78"/>
-      <c r="U11" s="76"/>
-      <c r="V11" s="76"/>
-      <c r="W11" s="76"/>
-      <c r="X11" s="77"/>
-      <c r="Y11" s="77"/>
-      <c r="Z11" s="77"/>
-      <c r="AA11" s="78"/>
-      <c r="AB11" s="76"/>
-      <c r="AC11" s="76"/>
-      <c r="AD11" t="s" s="79">
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="72"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="72"/>
+      <c r="U11" s="72"/>
+      <c r="V11" s="72"/>
+      <c r="W11" s="72"/>
+      <c r="X11" s="72"/>
+      <c r="Y11" s="72"/>
+      <c r="Z11" s="72"/>
+      <c r="AA11" s="72"/>
+      <c r="AB11" s="72"/>
+      <c r="AC11" s="72"/>
+      <c r="AD11" t="s" s="73">
         <v>0</v>
       </c>
-      <c r="AE11" t="s" s="80">
+      <c r="AE11" t="s" s="73">
         <v>0</v>
       </c>
-      <c r="AF11" t="s" s="80">
+      <c r="AF11" t="s" s="73">
         <v>0</v>
       </c>
-      <c r="AG11" t="s" s="80">
+      <c r="AG11" t="s" s="73">
         <v>0</v>
       </c>
-      <c r="AH11" s="81"/>
-      <c r="AI11" s="81"/>
-      <c r="AJ11" s="81"/>
-      <c r="AK11" s="81"/>
-      <c r="AL11" s="81"/>
-      <c r="AM11" s="81"/>
-      <c r="AN11" s="81"/>
-      <c r="AO11" s="81"/>
-      <c r="AP11" s="81"/>
-      <c r="AQ11" s="81"/>
-      <c r="AR11" s="81"/>
-      <c r="AS11" s="81"/>
-      <c r="AT11" s="81"/>
-      <c r="AU11" s="81"/>
-      <c r="AV11" s="81"/>
-      <c r="AW11" s="81"/>
+      <c r="AH11" s="74"/>
+      <c r="AI11" s="74"/>
+      <c r="AJ11" s="74"/>
+      <c r="AK11" s="74"/>
+      <c r="AL11" s="74"/>
+      <c r="AM11" s="74"/>
+      <c r="AN11" s="74"/>
+      <c r="AO11" s="74"/>
+      <c r="AP11" s="74"/>
+      <c r="AQ11" s="74"/>
+      <c r="AR11" s="74"/>
+      <c r="AS11" s="74"/>
+      <c r="AT11" s="74"/>
+      <c r="AU11" s="74"/>
+      <c r="AV11" s="74"/>
+      <c r="AW11" s="74"/>
     </row>
     <row r="12" ht="17.1" customHeight="1">
-      <c r="A12" t="s" s="82">
+      <c r="A12" t="s" s="75">
         <v>28</v>
       </c>
-      <c r="B12" t="s" s="65">
+      <c r="B12" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="67"/>
-      <c r="W12" s="67"/>
-      <c r="X12" s="68"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="68"/>
-      <c r="AF12" s="67"/>
-      <c r="AG12" s="67"/>
-      <c r="AH12" s="72"/>
-      <c r="AI12" s="72"/>
-      <c r="AJ12" s="72"/>
-      <c r="AK12" s="72"/>
-      <c r="AL12" s="72"/>
-      <c r="AM12" s="72"/>
-      <c r="AN12" s="72"/>
-      <c r="AO12" s="72"/>
-      <c r="AP12" s="72"/>
-      <c r="AQ12" s="72"/>
-      <c r="AR12" s="72"/>
-      <c r="AS12" s="72"/>
-      <c r="AT12" s="72"/>
-      <c r="AU12" s="72"/>
-      <c r="AV12" s="72"/>
-      <c r="AW12" s="72"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="65"/>
+      <c r="X12" s="65"/>
+      <c r="Y12" s="65"/>
+      <c r="Z12" s="65"/>
+      <c r="AA12" s="65"/>
+      <c r="AB12" s="65"/>
+      <c r="AC12" s="65"/>
+      <c r="AD12" s="65"/>
+      <c r="AE12" s="65"/>
+      <c r="AF12" s="65"/>
+      <c r="AG12" s="65"/>
+      <c r="AH12" s="68"/>
+      <c r="AI12" s="68"/>
+      <c r="AJ12" s="68"/>
+      <c r="AK12" s="68"/>
+      <c r="AL12" s="68"/>
+      <c r="AM12" s="68"/>
+      <c r="AN12" s="68"/>
+      <c r="AO12" s="68"/>
+      <c r="AP12" s="68"/>
+      <c r="AQ12" s="68"/>
+      <c r="AR12" s="68"/>
+      <c r="AS12" s="68"/>
+      <c r="AT12" s="68"/>
+      <c r="AU12" s="68"/>
+      <c r="AV12" s="68"/>
+      <c r="AW12" s="68"/>
     </row>
     <row r="13" ht="17.1" customHeight="1">
-      <c r="A13" s="74"/>
-      <c r="B13" t="s" s="75">
+      <c r="A13" s="70"/>
+      <c r="B13" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
-      <c r="Q13" s="78"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="76"/>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="77"/>
-      <c r="X13" s="78"/>
-      <c r="Y13" s="76"/>
-      <c r="Z13" s="76"/>
-      <c r="AA13" s="76"/>
-      <c r="AB13" s="77"/>
-      <c r="AC13" s="77"/>
-      <c r="AD13" s="77"/>
-      <c r="AE13" s="78"/>
-      <c r="AF13" s="77"/>
-      <c r="AG13" s="77"/>
-      <c r="AH13" s="81"/>
-      <c r="AI13" s="81"/>
-      <c r="AJ13" s="81"/>
-      <c r="AK13" s="81"/>
-      <c r="AL13" s="81"/>
-      <c r="AM13" s="81"/>
-      <c r="AN13" s="81"/>
-      <c r="AO13" s="81"/>
-      <c r="AP13" s="81"/>
-      <c r="AQ13" s="81"/>
-      <c r="AR13" s="81"/>
-      <c r="AS13" s="81"/>
-      <c r="AT13" s="81"/>
-      <c r="AU13" s="81"/>
-      <c r="AV13" s="81"/>
-      <c r="AW13" s="81"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72"/>
+      <c r="S13" s="72"/>
+      <c r="T13" s="72"/>
+      <c r="U13" s="72"/>
+      <c r="V13" s="72"/>
+      <c r="W13" s="72"/>
+      <c r="X13" s="72"/>
+      <c r="Y13" s="72"/>
+      <c r="Z13" s="72"/>
+      <c r="AA13" s="72"/>
+      <c r="AB13" s="72"/>
+      <c r="AC13" s="72"/>
+      <c r="AD13" s="72"/>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="72"/>
+      <c r="AG13" s="72"/>
+      <c r="AH13" s="74"/>
+      <c r="AI13" s="74"/>
+      <c r="AJ13" s="74"/>
+      <c r="AK13" s="74"/>
+      <c r="AL13" s="74"/>
+      <c r="AM13" s="74"/>
+      <c r="AN13" s="74"/>
+      <c r="AO13" s="74"/>
+      <c r="AP13" s="74"/>
+      <c r="AQ13" s="74"/>
+      <c r="AR13" s="74"/>
+      <c r="AS13" s="74"/>
+      <c r="AT13" s="74"/>
+      <c r="AU13" s="74"/>
+      <c r="AV13" s="74"/>
+      <c r="AW13" s="74"/>
     </row>
     <row r="14" ht="17.1" customHeight="1">
-      <c r="A14" t="s" s="82">
+      <c r="A14" t="s" s="75">
         <v>29</v>
       </c>
-      <c r="B14" t="s" s="65">
+      <c r="B14" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="66"/>
-      <c r="T14" s="66"/>
-      <c r="U14" s="67"/>
-      <c r="V14" s="67"/>
-      <c r="W14" s="68"/>
-      <c r="X14" s="66"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="66"/>
-      <c r="AA14" s="66"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="67"/>
-      <c r="AD14" s="68"/>
-      <c r="AE14" s="66"/>
-      <c r="AF14" s="68"/>
-      <c r="AG14" s="66"/>
-      <c r="AH14" s="72"/>
-      <c r="AI14" s="72"/>
-      <c r="AJ14" s="72"/>
-      <c r="AK14" s="72"/>
-      <c r="AL14" s="72"/>
-      <c r="AM14" s="72"/>
-      <c r="AN14" s="72"/>
-      <c r="AO14" s="72"/>
-      <c r="AP14" s="72"/>
-      <c r="AQ14" s="72"/>
-      <c r="AR14" s="72"/>
-      <c r="AS14" s="72"/>
-      <c r="AT14" s="72"/>
-      <c r="AU14" s="72"/>
-      <c r="AV14" s="72"/>
-      <c r="AW14" s="72"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65"/>
+      <c r="R14" s="65"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="65"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="65"/>
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="65"/>
+      <c r="AA14" s="65"/>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="65"/>
+      <c r="AD14" s="65"/>
+      <c r="AE14" s="65"/>
+      <c r="AF14" s="65"/>
+      <c r="AG14" s="65"/>
+      <c r="AH14" s="68"/>
+      <c r="AI14" s="68"/>
+      <c r="AJ14" s="68"/>
+      <c r="AK14" s="68"/>
+      <c r="AL14" s="68"/>
+      <c r="AM14" s="68"/>
+      <c r="AN14" s="68"/>
+      <c r="AO14" s="68"/>
+      <c r="AP14" s="68"/>
+      <c r="AQ14" s="68"/>
+      <c r="AR14" s="68"/>
+      <c r="AS14" s="68"/>
+      <c r="AT14" s="68"/>
+      <c r="AU14" s="68"/>
+      <c r="AV14" s="68"/>
+      <c r="AW14" s="68"/>
     </row>
     <row r="15" ht="17.1" customHeight="1">
-      <c r="A15" s="74"/>
-      <c r="B15" t="s" s="75">
+      <c r="A15" s="70"/>
+      <c r="B15" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="76"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="77"/>
-      <c r="W15" s="78"/>
-      <c r="X15" s="76"/>
-      <c r="Y15" s="78"/>
-      <c r="Z15" s="76"/>
-      <c r="AA15" s="76"/>
-      <c r="AB15" s="77"/>
-      <c r="AC15" s="77"/>
-      <c r="AD15" s="78"/>
-      <c r="AE15" s="76"/>
-      <c r="AF15" s="78"/>
-      <c r="AG15" s="76"/>
-      <c r="AH15" s="81"/>
-      <c r="AI15" s="81"/>
-      <c r="AJ15" s="81"/>
-      <c r="AK15" s="81"/>
-      <c r="AL15" s="81"/>
-      <c r="AM15" s="81"/>
-      <c r="AN15" s="81"/>
-      <c r="AO15" s="81"/>
-      <c r="AP15" s="81"/>
-      <c r="AQ15" s="81"/>
-      <c r="AR15" s="81"/>
-      <c r="AS15" s="81"/>
-      <c r="AT15" s="81"/>
-      <c r="AU15" s="81"/>
-      <c r="AV15" s="81"/>
-      <c r="AW15" s="81"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="72"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="72"/>
+      <c r="W15" s="72"/>
+      <c r="X15" s="72"/>
+      <c r="Y15" s="72"/>
+      <c r="Z15" s="72"/>
+      <c r="AA15" s="72"/>
+      <c r="AB15" s="72"/>
+      <c r="AC15" s="72"/>
+      <c r="AD15" s="72"/>
+      <c r="AE15" s="72"/>
+      <c r="AF15" s="72"/>
+      <c r="AG15" s="72"/>
+      <c r="AH15" s="74"/>
+      <c r="AI15" s="74"/>
+      <c r="AJ15" s="74"/>
+      <c r="AK15" s="74"/>
+      <c r="AL15" s="74"/>
+      <c r="AM15" s="74"/>
+      <c r="AN15" s="74"/>
+      <c r="AO15" s="74"/>
+      <c r="AP15" s="74"/>
+      <c r="AQ15" s="74"/>
+      <c r="AR15" s="74"/>
+      <c r="AS15" s="74"/>
+      <c r="AT15" s="74"/>
+      <c r="AU15" s="74"/>
+      <c r="AV15" s="74"/>
+      <c r="AW15" s="74"/>
     </row>
     <row r="16" ht="17.1" customHeight="1">
-      <c r="A16" t="s" s="82">
+      <c r="A16" t="s" s="75">
         <v>30</v>
       </c>
-      <c r="B16" t="s" s="65">
+      <c r="B16" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="67"/>
-      <c r="S16" s="67"/>
-      <c r="T16" s="68"/>
-      <c r="U16" s="66"/>
-      <c r="V16" s="68"/>
-      <c r="W16" s="66"/>
-      <c r="X16" s="66"/>
-      <c r="Y16" s="67"/>
-      <c r="Z16" s="67"/>
-      <c r="AA16" s="68"/>
-      <c r="AB16" s="66"/>
-      <c r="AC16" s="68"/>
-      <c r="AD16" s="66"/>
-      <c r="AE16" s="66"/>
-      <c r="AF16" s="67"/>
-      <c r="AG16" s="67"/>
-      <c r="AH16" s="72"/>
-      <c r="AI16" s="72"/>
-      <c r="AJ16" s="72"/>
-      <c r="AK16" s="72"/>
-      <c r="AL16" s="72"/>
-      <c r="AM16" s="72"/>
-      <c r="AN16" s="72"/>
-      <c r="AO16" s="72"/>
-      <c r="AP16" s="72"/>
-      <c r="AQ16" s="72"/>
-      <c r="AR16" s="72"/>
-      <c r="AS16" s="72"/>
-      <c r="AT16" s="72"/>
-      <c r="AU16" s="72"/>
-      <c r="AV16" s="72"/>
-      <c r="AW16" s="72"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
+      <c r="O16" s="65"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="65"/>
+      <c r="T16" s="65"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="65"/>
+      <c r="AA16" s="65"/>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="65"/>
+      <c r="AD16" s="65"/>
+      <c r="AE16" s="65"/>
+      <c r="AF16" s="65"/>
+      <c r="AG16" s="65"/>
+      <c r="AH16" s="68"/>
+      <c r="AI16" s="68"/>
+      <c r="AJ16" s="68"/>
+      <c r="AK16" s="68"/>
+      <c r="AL16" s="68"/>
+      <c r="AM16" s="68"/>
+      <c r="AN16" s="68"/>
+      <c r="AO16" s="68"/>
+      <c r="AP16" s="68"/>
+      <c r="AQ16" s="68"/>
+      <c r="AR16" s="68"/>
+      <c r="AS16" s="68"/>
+      <c r="AT16" s="68"/>
+      <c r="AU16" s="68"/>
+      <c r="AV16" s="68"/>
+      <c r="AW16" s="68"/>
     </row>
     <row r="17" ht="17.1" customHeight="1">
-      <c r="A17" s="74"/>
-      <c r="B17" t="s" s="75">
+      <c r="A17" s="70"/>
+      <c r="B17" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="77"/>
-      <c r="S17" s="77"/>
-      <c r="T17" s="78"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="78"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="77"/>
-      <c r="AA17" s="78"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="78"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AF17" s="77"/>
-      <c r="AG17" s="77"/>
-      <c r="AH17" s="81"/>
-      <c r="AI17" s="81"/>
-      <c r="AJ17" s="81"/>
-      <c r="AK17" s="81"/>
-      <c r="AL17" s="81"/>
-      <c r="AM17" s="81"/>
-      <c r="AN17" s="81"/>
-      <c r="AO17" s="81"/>
-      <c r="AP17" s="81"/>
-      <c r="AQ17" s="81"/>
-      <c r="AR17" s="81"/>
-      <c r="AS17" s="81"/>
-      <c r="AT17" s="81"/>
-      <c r="AU17" s="81"/>
-      <c r="AV17" s="81"/>
-      <c r="AW17" s="81"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="72"/>
+      <c r="X17" s="72"/>
+      <c r="Y17" s="72"/>
+      <c r="Z17" s="72"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="72"/>
+      <c r="AC17" s="72"/>
+      <c r="AD17" s="72"/>
+      <c r="AE17" s="72"/>
+      <c r="AF17" s="72"/>
+      <c r="AG17" s="72"/>
+      <c r="AH17" s="74"/>
+      <c r="AI17" s="74"/>
+      <c r="AJ17" s="74"/>
+      <c r="AK17" s="74"/>
+      <c r="AL17" s="74"/>
+      <c r="AM17" s="74"/>
+      <c r="AN17" s="74"/>
+      <c r="AO17" s="74"/>
+      <c r="AP17" s="74"/>
+      <c r="AQ17" s="74"/>
+      <c r="AR17" s="74"/>
+      <c r="AS17" s="74"/>
+      <c r="AT17" s="74"/>
+      <c r="AU17" s="74"/>
+      <c r="AV17" s="74"/>
+      <c r="AW17" s="74"/>
     </row>
     <row r="18" ht="17.1" customHeight="1">
-      <c r="A18" t="s" s="82">
+      <c r="A18" t="s" s="75">
         <v>31</v>
       </c>
-      <c r="B18" t="s" s="65">
+      <c r="B18" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="66"/>
-      <c r="O18" s="66"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="68"/>
-      <c r="S18" s="66"/>
-      <c r="T18" s="68"/>
-      <c r="U18" s="66"/>
-      <c r="V18" s="66"/>
-      <c r="W18" s="67"/>
-      <c r="X18" s="67"/>
-      <c r="Y18" s="68"/>
-      <c r="Z18" s="66"/>
-      <c r="AA18" s="68"/>
-      <c r="AB18" s="66"/>
-      <c r="AC18" s="66"/>
-      <c r="AD18" s="67"/>
-      <c r="AE18" s="67"/>
-      <c r="AF18" s="68"/>
-      <c r="AG18" s="66"/>
-      <c r="AH18" s="72"/>
-      <c r="AI18" s="72"/>
-      <c r="AJ18" s="72"/>
-      <c r="AK18" s="72"/>
-      <c r="AL18" s="72"/>
-      <c r="AM18" s="72"/>
-      <c r="AN18" s="72"/>
-      <c r="AO18" s="72"/>
-      <c r="AP18" s="72"/>
-      <c r="AQ18" s="72"/>
-      <c r="AR18" s="72"/>
-      <c r="AS18" s="72"/>
-      <c r="AT18" s="72"/>
-      <c r="AU18" s="72"/>
-      <c r="AV18" s="72"/>
-      <c r="AW18" s="72"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="65"/>
+      <c r="T18" s="65"/>
+      <c r="U18" s="65"/>
+      <c r="V18" s="65"/>
+      <c r="W18" s="65"/>
+      <c r="X18" s="65"/>
+      <c r="Y18" s="65"/>
+      <c r="Z18" s="65"/>
+      <c r="AA18" s="65"/>
+      <c r="AB18" s="65"/>
+      <c r="AC18" s="65"/>
+      <c r="AD18" s="65"/>
+      <c r="AE18" s="65"/>
+      <c r="AF18" s="65"/>
+      <c r="AG18" s="65"/>
+      <c r="AH18" s="68"/>
+      <c r="AI18" s="68"/>
+      <c r="AJ18" s="68"/>
+      <c r="AK18" s="68"/>
+      <c r="AL18" s="68"/>
+      <c r="AM18" s="68"/>
+      <c r="AN18" s="68"/>
+      <c r="AO18" s="68"/>
+      <c r="AP18" s="68"/>
+      <c r="AQ18" s="68"/>
+      <c r="AR18" s="68"/>
+      <c r="AS18" s="68"/>
+      <c r="AT18" s="68"/>
+      <c r="AU18" s="68"/>
+      <c r="AV18" s="68"/>
+      <c r="AW18" s="68"/>
     </row>
     <row r="19" ht="17.1" customHeight="1">
-      <c r="A19" s="74"/>
-      <c r="B19" t="s" s="75">
+      <c r="A19" s="70"/>
+      <c r="B19" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="78"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="78"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="78"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="77"/>
-      <c r="X19" s="77"/>
-      <c r="Y19" s="78"/>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="78"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="77"/>
-      <c r="AE19" s="77"/>
-      <c r="AF19" s="78"/>
-      <c r="AG19" s="76"/>
-      <c r="AH19" s="81"/>
-      <c r="AI19" s="81"/>
-      <c r="AJ19" s="81"/>
-      <c r="AK19" s="81"/>
-      <c r="AL19" s="81"/>
-      <c r="AM19" s="81"/>
-      <c r="AN19" s="81"/>
-      <c r="AO19" s="81"/>
-      <c r="AP19" s="81"/>
-      <c r="AQ19" s="81"/>
-      <c r="AR19" s="81"/>
-      <c r="AS19" s="81"/>
-      <c r="AT19" s="81"/>
-      <c r="AU19" s="81"/>
-      <c r="AV19" s="81"/>
-      <c r="AW19" s="81"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="72"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="72"/>
+      <c r="Y19" s="72"/>
+      <c r="Z19" s="72"/>
+      <c r="AA19" s="72"/>
+      <c r="AB19" s="72"/>
+      <c r="AC19" s="72"/>
+      <c r="AD19" s="72"/>
+      <c r="AE19" s="72"/>
+      <c r="AF19" s="72"/>
+      <c r="AG19" s="72"/>
+      <c r="AH19" s="74"/>
+      <c r="AI19" s="74"/>
+      <c r="AJ19" s="74"/>
+      <c r="AK19" s="74"/>
+      <c r="AL19" s="74"/>
+      <c r="AM19" s="74"/>
+      <c r="AN19" s="74"/>
+      <c r="AO19" s="74"/>
+      <c r="AP19" s="74"/>
+      <c r="AQ19" s="74"/>
+      <c r="AR19" s="74"/>
+      <c r="AS19" s="74"/>
+      <c r="AT19" s="74"/>
+      <c r="AU19" s="74"/>
+      <c r="AV19" s="74"/>
+      <c r="AW19" s="74"/>
     </row>
     <row r="20" ht="17.1" customHeight="1">
-      <c r="A20" t="s" s="82">
+      <c r="A20" t="s" s="75">
         <v>32</v>
       </c>
-      <c r="B20" t="s" s="65">
+      <c r="B20" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="66"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="66"/>
-      <c r="S20" s="66"/>
-      <c r="T20" s="67"/>
-      <c r="U20" s="67"/>
-      <c r="V20" s="68"/>
-      <c r="W20" s="66"/>
-      <c r="X20" s="68"/>
-      <c r="Y20" s="66"/>
-      <c r="Z20" s="66"/>
-      <c r="AA20" s="67"/>
-      <c r="AB20" s="67"/>
-      <c r="AC20" s="68"/>
-      <c r="AD20" s="66"/>
-      <c r="AE20" s="68"/>
-      <c r="AF20" s="66"/>
-      <c r="AG20" s="67"/>
-      <c r="AH20" s="72"/>
-      <c r="AI20" s="72"/>
-      <c r="AJ20" s="72"/>
-      <c r="AK20" s="72"/>
-      <c r="AL20" s="72"/>
-      <c r="AM20" s="72"/>
-      <c r="AN20" s="72"/>
-      <c r="AO20" s="72"/>
-      <c r="AP20" s="72"/>
-      <c r="AQ20" s="72"/>
-      <c r="AR20" s="72"/>
-      <c r="AS20" s="72"/>
-      <c r="AT20" s="72"/>
-      <c r="AU20" s="72"/>
-      <c r="AV20" s="72"/>
-      <c r="AW20" s="72"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
+      <c r="U20" s="65"/>
+      <c r="V20" s="65"/>
+      <c r="W20" s="65"/>
+      <c r="X20" s="65"/>
+      <c r="Y20" s="65"/>
+      <c r="Z20" s="65"/>
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="65"/>
+      <c r="AC20" s="65"/>
+      <c r="AD20" s="65"/>
+      <c r="AE20" s="65"/>
+      <c r="AF20" s="65"/>
+      <c r="AG20" s="65"/>
+      <c r="AH20" s="68"/>
+      <c r="AI20" s="68"/>
+      <c r="AJ20" s="68"/>
+      <c r="AK20" s="68"/>
+      <c r="AL20" s="68"/>
+      <c r="AM20" s="68"/>
+      <c r="AN20" s="68"/>
+      <c r="AO20" s="68"/>
+      <c r="AP20" s="68"/>
+      <c r="AQ20" s="68"/>
+      <c r="AR20" s="68"/>
+      <c r="AS20" s="68"/>
+      <c r="AT20" s="68"/>
+      <c r="AU20" s="68"/>
+      <c r="AV20" s="68"/>
+      <c r="AW20" s="68"/>
     </row>
     <row r="21" ht="17.1" customHeight="1">
-      <c r="A21" s="74"/>
-      <c r="B21" t="s" s="75">
+      <c r="A21" s="70"/>
+      <c r="B21" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="78"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="76"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="77"/>
-      <c r="V21" s="78"/>
-      <c r="W21" s="76"/>
-      <c r="X21" s="78"/>
-      <c r="Y21" s="76"/>
-      <c r="Z21" s="76"/>
-      <c r="AA21" s="77"/>
-      <c r="AB21" s="77"/>
-      <c r="AC21" s="78"/>
-      <c r="AD21" s="76"/>
-      <c r="AE21" s="78"/>
-      <c r="AF21" s="76"/>
-      <c r="AG21" s="77"/>
-      <c r="AH21" s="81"/>
-      <c r="AI21" s="81"/>
-      <c r="AJ21" s="81"/>
-      <c r="AK21" s="81"/>
-      <c r="AL21" s="81"/>
-      <c r="AM21" s="81"/>
-      <c r="AN21" s="81"/>
-      <c r="AO21" s="81"/>
-      <c r="AP21" s="81"/>
-      <c r="AQ21" s="81"/>
-      <c r="AR21" s="81"/>
-      <c r="AS21" s="81"/>
-      <c r="AT21" s="81"/>
-      <c r="AU21" s="81"/>
-      <c r="AV21" s="81"/>
-      <c r="AW21" s="81"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="72"/>
+      <c r="Y21" s="72"/>
+      <c r="Z21" s="72"/>
+      <c r="AA21" s="72"/>
+      <c r="AB21" s="72"/>
+      <c r="AC21" s="72"/>
+      <c r="AD21" s="72"/>
+      <c r="AE21" s="72"/>
+      <c r="AF21" s="72"/>
+      <c r="AG21" s="72"/>
+      <c r="AH21" s="74"/>
+      <c r="AI21" s="74"/>
+      <c r="AJ21" s="74"/>
+      <c r="AK21" s="74"/>
+      <c r="AL21" s="74"/>
+      <c r="AM21" s="74"/>
+      <c r="AN21" s="74"/>
+      <c r="AO21" s="74"/>
+      <c r="AP21" s="74"/>
+      <c r="AQ21" s="74"/>
+      <c r="AR21" s="74"/>
+      <c r="AS21" s="74"/>
+      <c r="AT21" s="74"/>
+      <c r="AU21" s="74"/>
+      <c r="AV21" s="74"/>
+      <c r="AW21" s="74"/>
     </row>
     <row r="22" ht="17.1" customHeight="1">
-      <c r="A22" t="s" s="82">
+      <c r="A22" t="s" s="75">
         <v>33</v>
       </c>
-      <c r="B22" t="s" s="65">
+      <c r="B22" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="68"/>
-      <c r="U22" s="66"/>
-      <c r="V22" s="68"/>
-      <c r="W22" s="66"/>
-      <c r="X22" s="66"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="68"/>
-      <c r="AB22" s="66"/>
-      <c r="AC22" s="68"/>
-      <c r="AD22" s="66"/>
-      <c r="AE22" s="66"/>
-      <c r="AF22" s="67"/>
-      <c r="AG22" s="67"/>
-      <c r="AH22" s="72"/>
-      <c r="AI22" s="72"/>
-      <c r="AJ22" s="72"/>
-      <c r="AK22" s="72"/>
-      <c r="AL22" s="72"/>
-      <c r="AM22" s="72"/>
-      <c r="AN22" s="72"/>
-      <c r="AO22" s="72"/>
-      <c r="AP22" s="72"/>
-      <c r="AQ22" s="72"/>
-      <c r="AR22" s="72"/>
-      <c r="AS22" s="72"/>
-      <c r="AT22" s="72"/>
-      <c r="AU22" s="72"/>
-      <c r="AV22" s="72"/>
-      <c r="AW22" s="72"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="65"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="65"/>
+      <c r="U22" s="65"/>
+      <c r="V22" s="65"/>
+      <c r="W22" s="65"/>
+      <c r="X22" s="65"/>
+      <c r="Y22" s="65"/>
+      <c r="Z22" s="65"/>
+      <c r="AA22" s="65"/>
+      <c r="AB22" s="65"/>
+      <c r="AC22" s="65"/>
+      <c r="AD22" s="65"/>
+      <c r="AE22" s="65"/>
+      <c r="AF22" s="65"/>
+      <c r="AG22" s="65"/>
+      <c r="AH22" s="68"/>
+      <c r="AI22" s="68"/>
+      <c r="AJ22" s="68"/>
+      <c r="AK22" s="68"/>
+      <c r="AL22" s="68"/>
+      <c r="AM22" s="68"/>
+      <c r="AN22" s="68"/>
+      <c r="AO22" s="68"/>
+      <c r="AP22" s="68"/>
+      <c r="AQ22" s="68"/>
+      <c r="AR22" s="68"/>
+      <c r="AS22" s="68"/>
+      <c r="AT22" s="68"/>
+      <c r="AU22" s="68"/>
+      <c r="AV22" s="68"/>
+      <c r="AW22" s="68"/>
     </row>
     <row r="23" ht="17.1" customHeight="1">
-      <c r="A23" s="74"/>
-      <c r="B23" t="s" s="75">
+      <c r="A23" s="70"/>
+      <c r="B23" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="78"/>
-      <c r="U23" s="76"/>
-      <c r="V23" s="78"/>
-      <c r="W23" s="76"/>
-      <c r="X23" s="76"/>
-      <c r="Y23" s="77"/>
-      <c r="Z23" s="77"/>
-      <c r="AA23" s="78"/>
-      <c r="AB23" s="76"/>
-      <c r="AC23" s="78"/>
-      <c r="AD23" s="76"/>
-      <c r="AE23" s="76"/>
-      <c r="AF23" s="77"/>
-      <c r="AG23" s="77"/>
-      <c r="AH23" s="81"/>
-      <c r="AI23" s="81"/>
-      <c r="AJ23" s="81"/>
-      <c r="AK23" s="81"/>
-      <c r="AL23" s="81"/>
-      <c r="AM23" s="81"/>
-      <c r="AN23" s="81"/>
-      <c r="AO23" s="81"/>
-      <c r="AP23" s="81"/>
-      <c r="AQ23" s="81"/>
-      <c r="AR23" s="81"/>
-      <c r="AS23" s="81"/>
-      <c r="AT23" s="81"/>
-      <c r="AU23" s="81"/>
-      <c r="AV23" s="81"/>
-      <c r="AW23" s="81"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="72"/>
+      <c r="S23" s="72"/>
+      <c r="T23" s="72"/>
+      <c r="U23" s="72"/>
+      <c r="V23" s="72"/>
+      <c r="W23" s="72"/>
+      <c r="X23" s="72"/>
+      <c r="Y23" s="72"/>
+      <c r="Z23" s="72"/>
+      <c r="AA23" s="72"/>
+      <c r="AB23" s="72"/>
+      <c r="AC23" s="72"/>
+      <c r="AD23" s="72"/>
+      <c r="AE23" s="72"/>
+      <c r="AF23" s="72"/>
+      <c r="AG23" s="72"/>
+      <c r="AH23" s="74"/>
+      <c r="AI23" s="74"/>
+      <c r="AJ23" s="74"/>
+      <c r="AK23" s="74"/>
+      <c r="AL23" s="74"/>
+      <c r="AM23" s="74"/>
+      <c r="AN23" s="74"/>
+      <c r="AO23" s="74"/>
+      <c r="AP23" s="74"/>
+      <c r="AQ23" s="74"/>
+      <c r="AR23" s="74"/>
+      <c r="AS23" s="74"/>
+      <c r="AT23" s="74"/>
+      <c r="AU23" s="74"/>
+      <c r="AV23" s="74"/>
+      <c r="AW23" s="74"/>
     </row>
     <row r="24" ht="17.1" customHeight="1">
-      <c r="A24" t="s" s="82">
+      <c r="A24" t="s" s="75">
         <v>34</v>
       </c>
-      <c r="B24" t="s" s="65">
+      <c r="B24" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="66"/>
-      <c r="N24" s="66"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="66"/>
-      <c r="S24" s="68"/>
-      <c r="T24" s="66"/>
-      <c r="U24" s="66"/>
-      <c r="V24" s="67"/>
-      <c r="W24" s="67"/>
-      <c r="X24" s="68"/>
-      <c r="Y24" s="66"/>
-      <c r="Z24" s="68"/>
-      <c r="AA24" s="66"/>
-      <c r="AB24" s="66"/>
-      <c r="AC24" s="67"/>
-      <c r="AD24" s="67"/>
-      <c r="AE24" s="68"/>
-      <c r="AF24" s="66"/>
-      <c r="AG24" s="68"/>
-      <c r="AH24" s="72"/>
-      <c r="AI24" s="72"/>
-      <c r="AJ24" s="72"/>
-      <c r="AK24" s="72"/>
-      <c r="AL24" s="72"/>
-      <c r="AM24" s="72"/>
-      <c r="AN24" s="72"/>
-      <c r="AO24" s="72"/>
-      <c r="AP24" s="72"/>
-      <c r="AQ24" s="72"/>
-      <c r="AR24" s="72"/>
-      <c r="AS24" s="72"/>
-      <c r="AT24" s="72"/>
-      <c r="AU24" s="72"/>
-      <c r="AV24" s="72"/>
-      <c r="AW24" s="72"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="65"/>
+      <c r="T24" s="65"/>
+      <c r="U24" s="65"/>
+      <c r="V24" s="65"/>
+      <c r="W24" s="65"/>
+      <c r="X24" s="65"/>
+      <c r="Y24" s="65"/>
+      <c r="Z24" s="65"/>
+      <c r="AA24" s="65"/>
+      <c r="AB24" s="65"/>
+      <c r="AC24" s="65"/>
+      <c r="AD24" s="65"/>
+      <c r="AE24" s="65"/>
+      <c r="AF24" s="65"/>
+      <c r="AG24" s="65"/>
+      <c r="AH24" s="68"/>
+      <c r="AI24" s="68"/>
+      <c r="AJ24" s="68"/>
+      <c r="AK24" s="68"/>
+      <c r="AL24" s="68"/>
+      <c r="AM24" s="68"/>
+      <c r="AN24" s="68"/>
+      <c r="AO24" s="68"/>
+      <c r="AP24" s="68"/>
+      <c r="AQ24" s="68"/>
+      <c r="AR24" s="68"/>
+      <c r="AS24" s="68"/>
+      <c r="AT24" s="68"/>
+      <c r="AU24" s="68"/>
+      <c r="AV24" s="68"/>
+      <c r="AW24" s="68"/>
     </row>
     <row r="25" ht="17.1" customHeight="1">
-      <c r="A25" s="74"/>
-      <c r="B25" t="s" s="75">
+      <c r="A25" s="70"/>
+      <c r="B25" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="76"/>
-      <c r="S25" s="78"/>
-      <c r="T25" s="76"/>
-      <c r="U25" s="76"/>
-      <c r="V25" s="77"/>
-      <c r="W25" s="77"/>
-      <c r="X25" s="78"/>
-      <c r="Y25" s="76"/>
-      <c r="Z25" s="78"/>
-      <c r="AA25" s="76"/>
-      <c r="AB25" s="76"/>
-      <c r="AC25" s="77"/>
-      <c r="AD25" s="77"/>
-      <c r="AE25" s="78"/>
-      <c r="AF25" s="76"/>
-      <c r="AG25" s="78"/>
-      <c r="AH25" s="81"/>
-      <c r="AI25" s="81"/>
-      <c r="AJ25" s="81"/>
-      <c r="AK25" s="81"/>
-      <c r="AL25" s="81"/>
-      <c r="AM25" s="81"/>
-      <c r="AN25" s="81"/>
-      <c r="AO25" s="81"/>
-      <c r="AP25" s="81"/>
-      <c r="AQ25" s="81"/>
-      <c r="AR25" s="81"/>
-      <c r="AS25" s="81"/>
-      <c r="AT25" s="81"/>
-      <c r="AU25" s="81"/>
-      <c r="AV25" s="81"/>
-      <c r="AW25" s="81"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="72"/>
+      <c r="Q25" s="72"/>
+      <c r="R25" s="72"/>
+      <c r="S25" s="72"/>
+      <c r="T25" s="72"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="72"/>
+      <c r="W25" s="72"/>
+      <c r="X25" s="72"/>
+      <c r="Y25" s="72"/>
+      <c r="Z25" s="72"/>
+      <c r="AA25" s="72"/>
+      <c r="AB25" s="72"/>
+      <c r="AC25" s="72"/>
+      <c r="AD25" s="72"/>
+      <c r="AE25" s="72"/>
+      <c r="AF25" s="72"/>
+      <c r="AG25" s="72"/>
+      <c r="AH25" s="74"/>
+      <c r="AI25" s="74"/>
+      <c r="AJ25" s="74"/>
+      <c r="AK25" s="74"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="74"/>
+      <c r="AN25" s="74"/>
+      <c r="AO25" s="74"/>
+      <c r="AP25" s="74"/>
+      <c r="AQ25" s="74"/>
+      <c r="AR25" s="74"/>
+      <c r="AS25" s="74"/>
+      <c r="AT25" s="74"/>
+      <c r="AU25" s="74"/>
+      <c r="AV25" s="74"/>
+      <c r="AW25" s="74"/>
     </row>
     <row r="26" ht="17.1" customHeight="1">
-      <c r="A26" t="s" s="82">
+      <c r="A26" t="s" s="75">
         <v>35</v>
       </c>
-      <c r="B26" t="s" s="65">
+      <c r="B26" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="67"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="66"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="66"/>
-      <c r="R26" s="66"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="67"/>
-      <c r="U26" s="68"/>
-      <c r="V26" s="66"/>
-      <c r="W26" s="68"/>
-      <c r="X26" s="66"/>
-      <c r="Y26" s="66"/>
-      <c r="Z26" s="67"/>
-      <c r="AA26" s="67"/>
-      <c r="AB26" s="68"/>
-      <c r="AC26" s="66"/>
-      <c r="AD26" s="68"/>
-      <c r="AE26" s="66"/>
-      <c r="AF26" s="66"/>
-      <c r="AG26" s="67"/>
-      <c r="AH26" s="72"/>
-      <c r="AI26" s="72"/>
-      <c r="AJ26" s="72"/>
-      <c r="AK26" s="72"/>
-      <c r="AL26" s="72"/>
-      <c r="AM26" s="72"/>
-      <c r="AN26" s="72"/>
-      <c r="AO26" s="72"/>
-      <c r="AP26" s="72"/>
-      <c r="AQ26" s="72"/>
-      <c r="AR26" s="72"/>
-      <c r="AS26" s="72"/>
-      <c r="AT26" s="72"/>
-      <c r="AU26" s="72"/>
-      <c r="AV26" s="72"/>
-      <c r="AW26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="65"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="65"/>
+      <c r="X26" s="65"/>
+      <c r="Y26" s="65"/>
+      <c r="Z26" s="65"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
+      <c r="AD26" s="65"/>
+      <c r="AE26" s="65"/>
+      <c r="AF26" s="65"/>
+      <c r="AG26" s="65"/>
+      <c r="AH26" s="68"/>
+      <c r="AI26" s="68"/>
+      <c r="AJ26" s="68"/>
+      <c r="AK26" s="68"/>
+      <c r="AL26" s="68"/>
+      <c r="AM26" s="68"/>
+      <c r="AN26" s="68"/>
+      <c r="AO26" s="68"/>
+      <c r="AP26" s="68"/>
+      <c r="AQ26" s="68"/>
+      <c r="AR26" s="68"/>
+      <c r="AS26" s="68"/>
+      <c r="AT26" s="68"/>
+      <c r="AU26" s="68"/>
+      <c r="AV26" s="68"/>
+      <c r="AW26" s="68"/>
     </row>
     <row r="27" ht="17.1" customHeight="1">
-      <c r="A27" s="74"/>
-      <c r="B27" t="s" s="75">
+      <c r="A27" s="70"/>
+      <c r="B27" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="78"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
-      <c r="S27" s="77"/>
-      <c r="T27" s="77"/>
-      <c r="U27" s="78"/>
-      <c r="V27" s="76"/>
-      <c r="W27" s="78"/>
-      <c r="X27" s="76"/>
-      <c r="Y27" s="76"/>
-      <c r="Z27" s="77"/>
-      <c r="AA27" s="77"/>
-      <c r="AB27" s="78"/>
-      <c r="AC27" s="76"/>
-      <c r="AD27" s="78"/>
-      <c r="AE27" s="76"/>
-      <c r="AF27" s="76"/>
-      <c r="AG27" s="77"/>
-      <c r="AH27" s="81"/>
-      <c r="AI27" s="81"/>
-      <c r="AJ27" s="81"/>
-      <c r="AK27" s="81"/>
-      <c r="AL27" s="81"/>
-      <c r="AM27" s="81"/>
-      <c r="AN27" s="81"/>
-      <c r="AO27" s="81"/>
-      <c r="AP27" s="81"/>
-      <c r="AQ27" s="81"/>
-      <c r="AR27" s="81"/>
-      <c r="AS27" s="81"/>
-      <c r="AT27" s="81"/>
-      <c r="AU27" s="81"/>
-      <c r="AV27" s="81"/>
-      <c r="AW27" s="81"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="72"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
+      <c r="W27" s="72"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="72"/>
+      <c r="Z27" s="72"/>
+      <c r="AA27" s="72"/>
+      <c r="AB27" s="72"/>
+      <c r="AC27" s="72"/>
+      <c r="AD27" s="72"/>
+      <c r="AE27" s="72"/>
+      <c r="AF27" s="72"/>
+      <c r="AG27" s="72"/>
+      <c r="AH27" s="74"/>
+      <c r="AI27" s="74"/>
+      <c r="AJ27" s="74"/>
+      <c r="AK27" s="74"/>
+      <c r="AL27" s="74"/>
+      <c r="AM27" s="74"/>
+      <c r="AN27" s="74"/>
+      <c r="AO27" s="74"/>
+      <c r="AP27" s="74"/>
+      <c r="AQ27" s="74"/>
+      <c r="AR27" s="74"/>
+      <c r="AS27" s="74"/>
+      <c r="AT27" s="74"/>
+      <c r="AU27" s="74"/>
+      <c r="AV27" s="74"/>
+      <c r="AW27" s="74"/>
     </row>
     <row r="28" ht="17.1" customHeight="1">
-      <c r="A28" t="s" s="82">
+      <c r="A28" t="s" s="75">
         <v>36</v>
       </c>
-      <c r="B28" t="s" s="65">
+      <c r="B28" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="66"/>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="68"/>
-      <c r="T28" s="66"/>
-      <c r="U28" s="68"/>
-      <c r="V28" s="66"/>
-      <c r="W28" s="66"/>
-      <c r="X28" s="67"/>
-      <c r="Y28" s="67"/>
-      <c r="Z28" s="68"/>
-      <c r="AA28" s="66"/>
-      <c r="AB28" s="68"/>
-      <c r="AC28" s="66"/>
-      <c r="AD28" s="66"/>
-      <c r="AE28" s="67"/>
-      <c r="AF28" s="67"/>
-      <c r="AG28" s="68"/>
-      <c r="AH28" s="72"/>
-      <c r="AI28" s="72"/>
-      <c r="AJ28" s="72"/>
-      <c r="AK28" s="72"/>
-      <c r="AL28" s="72"/>
-      <c r="AM28" s="72"/>
-      <c r="AN28" s="72"/>
-      <c r="AO28" s="72"/>
-      <c r="AP28" s="72"/>
-      <c r="AQ28" s="72"/>
-      <c r="AR28" s="72"/>
-      <c r="AS28" s="72"/>
-      <c r="AT28" s="72"/>
-      <c r="AU28" s="72"/>
-      <c r="AV28" s="72"/>
-      <c r="AW28" s="72"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
+      <c r="Y28" s="65"/>
+      <c r="Z28" s="65"/>
+      <c r="AA28" s="65"/>
+      <c r="AB28" s="65"/>
+      <c r="AC28" s="65"/>
+      <c r="AD28" s="65"/>
+      <c r="AE28" s="65"/>
+      <c r="AF28" s="65"/>
+      <c r="AG28" s="65"/>
+      <c r="AH28" s="68"/>
+      <c r="AI28" s="68"/>
+      <c r="AJ28" s="68"/>
+      <c r="AK28" s="68"/>
+      <c r="AL28" s="68"/>
+      <c r="AM28" s="68"/>
+      <c r="AN28" s="68"/>
+      <c r="AO28" s="68"/>
+      <c r="AP28" s="68"/>
+      <c r="AQ28" s="68"/>
+      <c r="AR28" s="68"/>
+      <c r="AS28" s="68"/>
+      <c r="AT28" s="68"/>
+      <c r="AU28" s="68"/>
+      <c r="AV28" s="68"/>
+      <c r="AW28" s="68"/>
     </row>
     <row r="29" ht="17.1" customHeight="1">
-      <c r="A29" s="74"/>
-      <c r="B29" t="s" s="75">
+      <c r="A29" s="70"/>
+      <c r="B29" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C29" s="77"/>
-      <c r="D29" s="77"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="78"/>
-      <c r="O29" s="76"/>
-      <c r="P29" s="76"/>
-      <c r="Q29" s="77"/>
-      <c r="R29" s="77"/>
-      <c r="S29" s="78"/>
-      <c r="T29" s="76"/>
-      <c r="U29" s="78"/>
-      <c r="V29" s="76"/>
-      <c r="W29" s="76"/>
-      <c r="X29" s="77"/>
-      <c r="Y29" s="77"/>
-      <c r="Z29" s="78"/>
-      <c r="AA29" s="76"/>
-      <c r="AB29" s="78"/>
-      <c r="AC29" s="76"/>
-      <c r="AD29" s="76"/>
-      <c r="AE29" s="77"/>
-      <c r="AF29" s="77"/>
-      <c r="AG29" s="78"/>
-      <c r="AH29" s="81"/>
-      <c r="AI29" s="81"/>
-      <c r="AJ29" s="81"/>
-      <c r="AK29" s="81"/>
-      <c r="AL29" s="81"/>
-      <c r="AM29" s="81"/>
-      <c r="AN29" s="81"/>
-      <c r="AO29" s="81"/>
-      <c r="AP29" s="81"/>
-      <c r="AQ29" s="81"/>
-      <c r="AR29" s="81"/>
-      <c r="AS29" s="81"/>
-      <c r="AT29" s="81"/>
-      <c r="AU29" s="81"/>
-      <c r="AV29" s="81"/>
-      <c r="AW29" s="81"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="72"/>
+      <c r="R29" s="72"/>
+      <c r="S29" s="72"/>
+      <c r="T29" s="72"/>
+      <c r="U29" s="72"/>
+      <c r="V29" s="72"/>
+      <c r="W29" s="72"/>
+      <c r="X29" s="72"/>
+      <c r="Y29" s="72"/>
+      <c r="Z29" s="72"/>
+      <c r="AA29" s="72"/>
+      <c r="AB29" s="72"/>
+      <c r="AC29" s="72"/>
+      <c r="AD29" s="72"/>
+      <c r="AE29" s="72"/>
+      <c r="AF29" s="72"/>
+      <c r="AG29" s="72"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="74"/>
+      <c r="AJ29" s="74"/>
+      <c r="AK29" s="74"/>
+      <c r="AL29" s="74"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="74"/>
+      <c r="AO29" s="74"/>
+      <c r="AP29" s="74"/>
+      <c r="AQ29" s="74"/>
+      <c r="AR29" s="74"/>
+      <c r="AS29" s="74"/>
+      <c r="AT29" s="74"/>
+      <c r="AU29" s="74"/>
+      <c r="AV29" s="74"/>
+      <c r="AW29" s="74"/>
     </row>
     <row r="30" ht="17.1" customHeight="1">
-      <c r="A30" t="s" s="82">
+      <c r="A30" t="s" s="75">
         <v>37</v>
       </c>
-      <c r="B30" t="s" s="65">
+      <c r="B30" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="66"/>
-      <c r="N30" s="67"/>
-      <c r="O30" s="67"/>
-      <c r="P30" s="68"/>
-      <c r="Q30" s="66"/>
-      <c r="R30" s="68"/>
-      <c r="S30" s="66"/>
-      <c r="T30" s="66"/>
-      <c r="U30" s="67"/>
-      <c r="V30" s="67"/>
-      <c r="W30" s="68"/>
-      <c r="X30" s="66"/>
-      <c r="Y30" s="68"/>
-      <c r="Z30" s="66"/>
-      <c r="AA30" s="66"/>
-      <c r="AB30" s="67"/>
-      <c r="AC30" s="67"/>
-      <c r="AD30" s="68"/>
-      <c r="AE30" s="66"/>
-      <c r="AF30" s="68"/>
-      <c r="AG30" s="67"/>
-      <c r="AH30" s="72"/>
-      <c r="AI30" s="72"/>
-      <c r="AJ30" s="72"/>
-      <c r="AK30" s="72"/>
-      <c r="AL30" s="72"/>
-      <c r="AM30" s="72"/>
-      <c r="AN30" s="72"/>
-      <c r="AO30" s="72"/>
-      <c r="AP30" s="72"/>
-      <c r="AQ30" s="72"/>
-      <c r="AR30" s="72"/>
-      <c r="AS30" s="72"/>
-      <c r="AT30" s="72"/>
-      <c r="AU30" s="72"/>
-      <c r="AV30" s="72"/>
-      <c r="AW30" s="72"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="65"/>
+      <c r="U30" s="65"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="65"/>
+      <c r="X30" s="65"/>
+      <c r="Y30" s="65"/>
+      <c r="Z30" s="65"/>
+      <c r="AA30" s="65"/>
+      <c r="AB30" s="65"/>
+      <c r="AC30" s="65"/>
+      <c r="AD30" s="65"/>
+      <c r="AE30" s="65"/>
+      <c r="AF30" s="65"/>
+      <c r="AG30" s="65"/>
+      <c r="AH30" s="68"/>
+      <c r="AI30" s="68"/>
+      <c r="AJ30" s="68"/>
+      <c r="AK30" s="68"/>
+      <c r="AL30" s="68"/>
+      <c r="AM30" s="68"/>
+      <c r="AN30" s="68"/>
+      <c r="AO30" s="68"/>
+      <c r="AP30" s="68"/>
+      <c r="AQ30" s="68"/>
+      <c r="AR30" s="68"/>
+      <c r="AS30" s="68"/>
+      <c r="AT30" s="68"/>
+      <c r="AU30" s="68"/>
+      <c r="AV30" s="68"/>
+      <c r="AW30" s="68"/>
     </row>
     <row r="31" ht="17.1" customHeight="1">
-      <c r="A31" s="74"/>
-      <c r="B31" t="s" s="75">
+      <c r="A31" s="70"/>
+      <c r="B31" t="s" s="71">
         <v>27</v>
       </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="78"/>
-      <c r="S31" s="76"/>
-      <c r="T31" s="76"/>
-      <c r="U31" s="77"/>
-      <c r="V31" s="77"/>
-      <c r="W31" s="78"/>
-      <c r="X31" s="76"/>
-      <c r="Y31" s="78"/>
-      <c r="Z31" s="76"/>
-      <c r="AA31" s="76"/>
-      <c r="AB31" s="77"/>
-      <c r="AC31" s="77"/>
-      <c r="AD31" s="78"/>
-      <c r="AE31" s="76"/>
-      <c r="AF31" s="78"/>
-      <c r="AG31" s="77"/>
-      <c r="AH31" s="81"/>
-      <c r="AI31" s="81"/>
-      <c r="AJ31" s="81"/>
-      <c r="AK31" s="81"/>
-      <c r="AL31" s="81"/>
-      <c r="AM31" s="81"/>
-      <c r="AN31" s="81"/>
-      <c r="AO31" s="81"/>
-      <c r="AP31" s="81"/>
-      <c r="AQ31" s="81"/>
-      <c r="AR31" s="81"/>
-      <c r="AS31" s="81"/>
-      <c r="AT31" s="81"/>
-      <c r="AU31" s="81"/>
-      <c r="AV31" s="81"/>
-      <c r="AW31" s="81"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
+      <c r="Q31" s="72"/>
+      <c r="R31" s="72"/>
+      <c r="S31" s="72"/>
+      <c r="T31" s="72"/>
+      <c r="U31" s="72"/>
+      <c r="V31" s="72"/>
+      <c r="W31" s="72"/>
+      <c r="X31" s="72"/>
+      <c r="Y31" s="72"/>
+      <c r="Z31" s="72"/>
+      <c r="AA31" s="72"/>
+      <c r="AB31" s="72"/>
+      <c r="AC31" s="72"/>
+      <c r="AD31" s="72"/>
+      <c r="AE31" s="72"/>
+      <c r="AF31" s="72"/>
+      <c r="AG31" s="72"/>
+      <c r="AH31" s="74"/>
+      <c r="AI31" s="74"/>
+      <c r="AJ31" s="74"/>
+      <c r="AK31" s="74"/>
+      <c r="AL31" s="74"/>
+      <c r="AM31" s="74"/>
+      <c r="AN31" s="74"/>
+      <c r="AO31" s="74"/>
+      <c r="AP31" s="74"/>
+      <c r="AQ31" s="74"/>
+      <c r="AR31" s="74"/>
+      <c r="AS31" s="74"/>
+      <c r="AT31" s="74"/>
+      <c r="AU31" s="74"/>
+      <c r="AV31" s="74"/>
+      <c r="AW31" s="74"/>
     </row>
     <row r="32" ht="17.1" customHeight="1">
-      <c r="A32" t="s" s="82">
+      <c r="A32" t="s" s="75">
         <v>38</v>
       </c>
-      <c r="B32" t="s" s="65">
+      <c r="B32" t="s" s="64">
         <v>26</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="67"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="66"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="66"/>
-      <c r="R32" s="66"/>
-      <c r="S32" s="67"/>
-      <c r="T32" s="67"/>
-      <c r="U32" s="68"/>
-      <c r="V32" s="66"/>
-      <c r="W32" s="68"/>
-      <c r="X32" s="66"/>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="67"/>
-      <c r="AA32" s="66"/>
-      <c r="AB32" s="66"/>
-      <c r="AC32" s="66"/>
-      <c r="AD32" s="68"/>
-      <c r="AE32" s="66"/>
-      <c r="AF32" s="66"/>
-      <c r="AG32" s="67"/>
-      <c r="AH32" s="72"/>
-      <c r="AI32" s="72"/>
-      <c r="AJ32" s="72"/>
-      <c r="AK32" s="72"/>
-      <c r="AL32" s="72"/>
-      <c r="AM32" s="72"/>
-      <c r="AN32" s="72"/>
-      <c r="AO32" s="72"/>
-      <c r="AP32" s="72"/>
-      <c r="AQ32" s="72"/>
-      <c r="AR32" s="72"/>
-      <c r="AS32" s="72"/>
-      <c r="AT32" s="72"/>
-      <c r="AU32" s="72"/>
-      <c r="AV32" s="72"/>
-      <c r="AW32" s="72"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="65"/>
+      <c r="S32" s="65"/>
+      <c r="T32" s="65"/>
+      <c r="U32" s="65"/>
+      <c r="V32" s="65"/>
+      <c r="W32" s="65"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="65"/>
+      <c r="Z32" s="65"/>
+      <c r="AA32" s="65"/>
+      <c r="AB32" s="65"/>
+      <c r="AC32" s="65"/>
+      <c r="AD32" s="65"/>
+      <c r="AE32" s="65"/>
+      <c r="AF32" s="65"/>
+      <c r="AG32" s="65"/>
+      <c r="AH32" s="68"/>
+      <c r="AI32" s="68"/>
+      <c r="AJ32" s="68"/>
+      <c r="AK32" s="68"/>
+      <c r="AL32" s="68"/>
+      <c r="AM32" s="68"/>
+      <c r="AN32" s="68"/>
+      <c r="AO32" s="68"/>
+      <c r="AP32" s="68"/>
+      <c r="AQ32" s="68"/>
+      <c r="AR32" s="68"/>
+      <c r="AS32" s="68"/>
+      <c r="AT32" s="68"/>
+      <c r="AU32" s="68"/>
+      <c r="AV32" s="68"/>
+      <c r="AW32" s="68"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="A33" s="83"/>
-      <c r="B33" t="s" s="84">
+      <c r="A33" s="76"/>
+      <c r="B33" t="s" s="77">
         <v>27</v>
       </c>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="87"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="85"/>
-      <c r="L33" s="86"/>
-      <c r="M33" s="86"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="85"/>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="85"/>
-      <c r="R33" s="85"/>
-      <c r="S33" s="86"/>
-      <c r="T33" s="86"/>
-      <c r="U33" s="87"/>
-      <c r="V33" s="85"/>
-      <c r="W33" s="87"/>
-      <c r="X33" s="85"/>
-      <c r="Y33" s="85"/>
-      <c r="Z33" s="86"/>
-      <c r="AA33" s="85"/>
-      <c r="AB33" s="85"/>
-      <c r="AC33" s="85"/>
-      <c r="AD33" s="87"/>
-      <c r="AE33" s="85"/>
-      <c r="AF33" s="85"/>
-      <c r="AG33" s="86"/>
-      <c r="AH33" s="88"/>
-      <c r="AI33" s="88"/>
-      <c r="AJ33" s="88"/>
-      <c r="AK33" s="88"/>
-      <c r="AL33" s="88"/>
-      <c r="AM33" s="88"/>
-      <c r="AN33" s="88"/>
-      <c r="AO33" s="88"/>
-      <c r="AP33" s="88"/>
-      <c r="AQ33" s="88"/>
-      <c r="AR33" s="88"/>
-      <c r="AS33" s="88"/>
-      <c r="AT33" s="88"/>
-      <c r="AU33" s="88"/>
-      <c r="AV33" s="88"/>
-      <c r="AW33" s="88"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
+      <c r="O33" s="78"/>
+      <c r="P33" s="78"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="78"/>
+      <c r="S33" s="78"/>
+      <c r="T33" s="78"/>
+      <c r="U33" s="78"/>
+      <c r="V33" s="78"/>
+      <c r="W33" s="78"/>
+      <c r="X33" s="78"/>
+      <c r="Y33" s="78"/>
+      <c r="Z33" s="78"/>
+      <c r="AA33" s="78"/>
+      <c r="AB33" s="78"/>
+      <c r="AC33" s="78"/>
+      <c r="AD33" s="78"/>
+      <c r="AE33" s="78"/>
+      <c r="AF33" s="78"/>
+      <c r="AG33" s="78"/>
+      <c r="AH33" s="79"/>
+      <c r="AI33" s="79"/>
+      <c r="AJ33" s="79"/>
+      <c r="AK33" s="79"/>
+      <c r="AL33" s="79"/>
+      <c r="AM33" s="79"/>
+      <c r="AN33" s="79"/>
+      <c r="AO33" s="79"/>
+      <c r="AP33" s="79"/>
+      <c r="AQ33" s="79"/>
+      <c r="AR33" s="79"/>
+      <c r="AS33" s="79"/>
+      <c r="AT33" s="79"/>
+      <c r="AU33" s="79"/>
+      <c r="AV33" s="79"/>
+      <c r="AW33" s="79"/>
     </row>
     <row r="34" ht="17.1" customHeight="1">
-      <c r="A34" t="s" s="89">
+      <c r="A34" t="s" s="80">
         <v>39</v>
       </c>
-      <c r="B34" s="90"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="92"/>
-      <c r="Q34" s="92"/>
-      <c r="R34" s="92"/>
-      <c r="S34" s="92"/>
-      <c r="T34" s="92"/>
-      <c r="U34" s="92"/>
-      <c r="V34" s="92"/>
-      <c r="W34" s="92"/>
-      <c r="X34" s="92"/>
-      <c r="Y34" s="92"/>
-      <c r="Z34" s="92"/>
-      <c r="AA34" s="92"/>
-      <c r="AB34" s="92"/>
-      <c r="AC34" s="92"/>
-      <c r="AD34" s="92"/>
-      <c r="AE34" s="92"/>
-      <c r="AF34" s="92"/>
-      <c r="AG34" s="93"/>
-      <c r="AH34" s="94"/>
-      <c r="AI34" s="92"/>
-      <c r="AJ34" s="92"/>
-      <c r="AK34" s="92"/>
-      <c r="AL34" s="93"/>
-      <c r="AM34" s="94"/>
-      <c r="AN34" s="92"/>
-      <c r="AO34" s="92"/>
-      <c r="AP34" s="93"/>
-      <c r="AQ34" s="94"/>
-      <c r="AR34" s="92"/>
-      <c r="AS34" s="93"/>
-      <c r="AT34" s="94"/>
-      <c r="AU34" s="92"/>
-      <c r="AV34" s="92"/>
-      <c r="AW34" s="93"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="83"/>
+      <c r="O34" s="83"/>
+      <c r="P34" s="83"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="83"/>
+      <c r="S34" s="83"/>
+      <c r="T34" s="83"/>
+      <c r="U34" s="83"/>
+      <c r="V34" s="83"/>
+      <c r="W34" s="83"/>
+      <c r="X34" s="83"/>
+      <c r="Y34" s="83"/>
+      <c r="Z34" s="83"/>
+      <c r="AA34" s="83"/>
+      <c r="AB34" s="83"/>
+      <c r="AC34" s="83"/>
+      <c r="AD34" s="83"/>
+      <c r="AE34" s="83"/>
+      <c r="AF34" s="83"/>
+      <c r="AG34" s="84"/>
+      <c r="AH34" s="85"/>
+      <c r="AI34" s="83"/>
+      <c r="AJ34" s="83"/>
+      <c r="AK34" s="83"/>
+      <c r="AL34" s="84"/>
+      <c r="AM34" s="85"/>
+      <c r="AN34" s="83"/>
+      <c r="AO34" s="83"/>
+      <c r="AP34" s="84"/>
+      <c r="AQ34" s="85"/>
+      <c r="AR34" s="83"/>
+      <c r="AS34" s="84"/>
+      <c r="AT34" s="85"/>
+      <c r="AU34" s="83"/>
+      <c r="AV34" s="83"/>
+      <c r="AW34" s="84"/>
     </row>
     <row r="35" ht="17.25" customHeight="1">
-      <c r="A35" s="95"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="95"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="95"/>
-      <c r="Q35" s="95"/>
-      <c r="R35" s="95"/>
-      <c r="S35" s="95"/>
-      <c r="T35" s="95"/>
-      <c r="U35" s="95"/>
-      <c r="V35" s="95"/>
-      <c r="W35" s="95"/>
-      <c r="X35" s="95"/>
-      <c r="Y35" s="95"/>
-      <c r="Z35" s="95"/>
-      <c r="AA35" s="95"/>
-      <c r="AB35" s="95"/>
-      <c r="AC35" s="95"/>
-      <c r="AD35" s="95"/>
-      <c r="AE35" s="95"/>
-      <c r="AF35" s="95"/>
-      <c r="AG35" s="95"/>
-      <c r="AH35" s="95"/>
-      <c r="AI35" s="95"/>
-      <c r="AJ35" s="95"/>
-      <c r="AK35" s="95"/>
-      <c r="AL35" s="95"/>
-      <c r="AM35" s="95"/>
-      <c r="AN35" s="95"/>
-      <c r="AO35" s="95"/>
-      <c r="AP35" s="95"/>
-      <c r="AQ35" s="95"/>
-      <c r="AR35" s="95"/>
-      <c r="AS35" s="95"/>
-      <c r="AT35" s="95"/>
-      <c r="AU35" s="95"/>
-      <c r="AV35" s="95"/>
-      <c r="AW35" s="96"/>
+      <c r="A35" s="86"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="86"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="86"/>
+      <c r="R35" s="86"/>
+      <c r="S35" s="86"/>
+      <c r="T35" s="86"/>
+      <c r="U35" s="86"/>
+      <c r="V35" s="86"/>
+      <c r="W35" s="86"/>
+      <c r="X35" s="86"/>
+      <c r="Y35" s="86"/>
+      <c r="Z35" s="86"/>
+      <c r="AA35" s="86"/>
+      <c r="AB35" s="86"/>
+      <c r="AC35" s="86"/>
+      <c r="AD35" s="86"/>
+      <c r="AE35" s="86"/>
+      <c r="AF35" s="86"/>
+      <c r="AG35" s="86"/>
+      <c r="AH35" s="86"/>
+      <c r="AI35" s="86"/>
+      <c r="AJ35" s="86"/>
+      <c r="AK35" s="86"/>
+      <c r="AL35" s="86"/>
+      <c r="AM35" s="86"/>
+      <c r="AN35" s="86"/>
+      <c r="AO35" s="86"/>
+      <c r="AP35" s="86"/>
+      <c r="AQ35" s="86"/>
+      <c r="AR35" s="86"/>
+      <c r="AS35" s="86"/>
+      <c r="AT35" s="86"/>
+      <c r="AU35" s="86"/>
+      <c r="AV35" s="86"/>
+      <c r="AW35" s="87"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" t="s" s="97">
+      <c r="A36" t="s" s="88">
         <v>40</v>
       </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
-      <c r="M36" s="98"/>
-      <c r="N36" s="98"/>
-      <c r="O36" s="98"/>
-      <c r="P36" s="98"/>
-      <c r="Q36" s="98"/>
-      <c r="R36" s="98"/>
-      <c r="S36" s="98"/>
-      <c r="T36" s="98"/>
-      <c r="U36" s="98"/>
-      <c r="V36" s="98"/>
-      <c r="W36" s="98"/>
-      <c r="X36" s="98"/>
-      <c r="Y36" s="98"/>
-      <c r="Z36" s="98"/>
-      <c r="AA36" s="98"/>
-      <c r="AB36" s="98"/>
-      <c r="AC36" s="98"/>
-      <c r="AD36" s="98"/>
-      <c r="AE36" s="98"/>
-      <c r="AF36" s="98"/>
-      <c r="AG36" s="98"/>
-      <c r="AH36" s="98"/>
-      <c r="AI36" s="98"/>
-      <c r="AJ36" s="98"/>
-      <c r="AK36" s="98"/>
-      <c r="AL36" s="98"/>
-      <c r="AM36" s="98"/>
-      <c r="AN36" s="98"/>
-      <c r="AO36" s="98"/>
-      <c r="AP36" s="98"/>
-      <c r="AQ36" s="98"/>
-      <c r="AR36" s="98"/>
-      <c r="AS36" s="98"/>
-      <c r="AT36" s="98"/>
-      <c r="AU36" s="98"/>
-      <c r="AV36" s="98"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="89"/>
+      <c r="M36" s="89"/>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
+      <c r="P36" s="89"/>
+      <c r="Q36" s="89"/>
+      <c r="R36" s="89"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="89"/>
+      <c r="U36" s="89"/>
+      <c r="V36" s="89"/>
+      <c r="W36" s="89"/>
+      <c r="X36" s="89"/>
+      <c r="Y36" s="89"/>
+      <c r="Z36" s="89"/>
+      <c r="AA36" s="89"/>
+      <c r="AB36" s="89"/>
+      <c r="AC36" s="89"/>
+      <c r="AD36" s="89"/>
+      <c r="AE36" s="89"/>
+      <c r="AF36" s="89"/>
+      <c r="AG36" s="89"/>
+      <c r="AH36" s="89"/>
+      <c r="AI36" s="89"/>
+      <c r="AJ36" s="89"/>
+      <c r="AK36" s="89"/>
+      <c r="AL36" s="89"/>
+      <c r="AM36" s="89"/>
+      <c r="AN36" s="89"/>
+      <c r="AO36" s="89"/>
+      <c r="AP36" s="89"/>
+      <c r="AQ36" s="89"/>
+      <c r="AR36" s="89"/>
+      <c r="AS36" s="89"/>
+      <c r="AT36" s="89"/>
+      <c r="AU36" s="89"/>
+      <c r="AV36" s="89"/>
       <c r="AW36" s="2"/>
     </row>
     <row r="37" ht="17.25" customHeight="1">
-      <c r="A37" s="98"/>
-      <c r="B37" s="98"/>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="98"/>
-      <c r="G37" s="98"/>
-      <c r="H37" s="98"/>
-      <c r="I37" s="98"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="98"/>
-      <c r="M37" s="98"/>
-      <c r="N37" s="98"/>
-      <c r="O37" s="98"/>
-      <c r="P37" s="98"/>
-      <c r="Q37" s="98"/>
-      <c r="R37" s="98"/>
-      <c r="S37" s="98"/>
-      <c r="T37" s="98"/>
-      <c r="U37" s="98"/>
-      <c r="V37" s="98"/>
-      <c r="W37" s="98"/>
-      <c r="X37" s="98"/>
-      <c r="Y37" s="98"/>
-      <c r="Z37" s="98"/>
-      <c r="AA37" s="98"/>
-      <c r="AB37" s="98"/>
-      <c r="AC37" s="98"/>
-      <c r="AD37" s="98"/>
-      <c r="AE37" s="98"/>
-      <c r="AF37" s="98"/>
-      <c r="AG37" s="98"/>
-      <c r="AH37" s="98"/>
-      <c r="AI37" s="98"/>
-      <c r="AJ37" s="98"/>
-      <c r="AK37" s="98"/>
-      <c r="AL37" s="98"/>
-      <c r="AM37" s="98"/>
-      <c r="AN37" s="98"/>
-      <c r="AO37" s="98"/>
-      <c r="AP37" s="98"/>
-      <c r="AQ37" s="98"/>
-      <c r="AR37" s="98"/>
-      <c r="AS37" s="98"/>
-      <c r="AT37" s="98"/>
-      <c r="AU37" s="98"/>
-      <c r="AV37" s="98"/>
+      <c r="A37" s="89"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="89"/>
+      <c r="N37" s="89"/>
+      <c r="O37" s="89"/>
+      <c r="P37" s="89"/>
+      <c r="Q37" s="89"/>
+      <c r="R37" s="89"/>
+      <c r="S37" s="89"/>
+      <c r="T37" s="89"/>
+      <c r="U37" s="89"/>
+      <c r="V37" s="89"/>
+      <c r="W37" s="89"/>
+      <c r="X37" s="89"/>
+      <c r="Y37" s="89"/>
+      <c r="Z37" s="89"/>
+      <c r="AA37" s="89"/>
+      <c r="AB37" s="89"/>
+      <c r="AC37" s="89"/>
+      <c r="AD37" s="89"/>
+      <c r="AE37" s="89"/>
+      <c r="AF37" s="89"/>
+      <c r="AG37" s="89"/>
+      <c r="AH37" s="89"/>
+      <c r="AI37" s="89"/>
+      <c r="AJ37" s="89"/>
+      <c r="AK37" s="89"/>
+      <c r="AL37" s="89"/>
+      <c r="AM37" s="89"/>
+      <c r="AN37" s="89"/>
+      <c r="AO37" s="89"/>
+      <c r="AP37" s="89"/>
+      <c r="AQ37" s="89"/>
+      <c r="AR37" s="89"/>
+      <c r="AS37" s="89"/>
+      <c r="AT37" s="89"/>
+      <c r="AU37" s="89"/>
+      <c r="AV37" s="89"/>
       <c r="AW37" s="2"/>
     </row>
     <row r="38" ht="8" customHeight="1">
-      <c r="A38" s="98"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="98"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="98"/>
-      <c r="O38" s="98"/>
-      <c r="P38" s="98"/>
-      <c r="Q38" s="98"/>
-      <c r="R38" s="98"/>
-      <c r="S38" s="98"/>
-      <c r="T38" s="98"/>
-      <c r="U38" s="98"/>
-      <c r="V38" s="98"/>
-      <c r="W38" s="98"/>
-      <c r="X38" s="98"/>
-      <c r="Y38" s="98"/>
-      <c r="Z38" s="98"/>
-      <c r="AA38" s="98"/>
-      <c r="AB38" s="98"/>
-      <c r="AC38" s="98"/>
-      <c r="AD38" s="98"/>
-      <c r="AE38" s="98"/>
-      <c r="AF38" s="98"/>
-      <c r="AG38" s="98"/>
-      <c r="AH38" s="98"/>
-      <c r="AI38" s="98"/>
-      <c r="AJ38" s="98"/>
-      <c r="AK38" s="98"/>
-      <c r="AL38" s="98"/>
-      <c r="AM38" s="98"/>
-      <c r="AN38" s="98"/>
-      <c r="AO38" s="98"/>
-      <c r="AP38" s="98"/>
-      <c r="AQ38" s="98"/>
-      <c r="AR38" s="98"/>
-      <c r="AS38" s="98"/>
-      <c r="AT38" s="98"/>
-      <c r="AU38" s="98"/>
-      <c r="AV38" s="98"/>
+      <c r="A38" s="89"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="89"/>
+      <c r="T38" s="89"/>
+      <c r="U38" s="89"/>
+      <c r="V38" s="89"/>
+      <c r="W38" s="89"/>
+      <c r="X38" s="89"/>
+      <c r="Y38" s="89"/>
+      <c r="Z38" s="89"/>
+      <c r="AA38" s="89"/>
+      <c r="AB38" s="89"/>
+      <c r="AC38" s="89"/>
+      <c r="AD38" s="89"/>
+      <c r="AE38" s="89"/>
+      <c r="AF38" s="89"/>
+      <c r="AG38" s="89"/>
+      <c r="AH38" s="89"/>
+      <c r="AI38" s="89"/>
+      <c r="AJ38" s="89"/>
+      <c r="AK38" s="89"/>
+      <c r="AL38" s="89"/>
+      <c r="AM38" s="89"/>
+      <c r="AN38" s="89"/>
+      <c r="AO38" s="89"/>
+      <c r="AP38" s="89"/>
+      <c r="AQ38" s="89"/>
+      <c r="AR38" s="89"/>
+      <c r="AS38" s="89"/>
+      <c r="AT38" s="89"/>
+      <c r="AU38" s="89"/>
+      <c r="AV38" s="89"/>
       <c r="AW38" s="2"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="99"/>
-      <c r="B39" s="99"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="90"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -4729,25 +4678,25 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2"/>
-      <c r="AE41" s="100"/>
-      <c r="AF41" s="100"/>
-      <c r="AG41" s="100"/>
-      <c r="AH41" s="100"/>
-      <c r="AI41" s="100"/>
-      <c r="AJ41" s="100"/>
-      <c r="AK41" s="100"/>
-      <c r="AL41" s="100"/>
-      <c r="AM41" s="100"/>
-      <c r="AN41" s="100"/>
-      <c r="AO41" s="100"/>
-      <c r="AP41" s="100"/>
-      <c r="AQ41" s="100"/>
-      <c r="AR41" s="100"/>
-      <c r="AS41" s="100"/>
-      <c r="AT41" s="100"/>
-      <c r="AU41" s="100"/>
-      <c r="AV41" s="100"/>
-      <c r="AW41" s="100"/>
+      <c r="AE41" s="91"/>
+      <c r="AF41" s="91"/>
+      <c r="AG41" s="91"/>
+      <c r="AH41" s="91"/>
+      <c r="AI41" s="91"/>
+      <c r="AJ41" s="91"/>
+      <c r="AK41" s="91"/>
+      <c r="AL41" s="91"/>
+      <c r="AM41" s="91"/>
+      <c r="AN41" s="91"/>
+      <c r="AO41" s="91"/>
+      <c r="AP41" s="91"/>
+      <c r="AQ41" s="91"/>
+      <c r="AR41" s="91"/>
+      <c r="AS41" s="91"/>
+      <c r="AT41" s="91"/>
+      <c r="AU41" s="91"/>
+      <c r="AV41" s="91"/>
+      <c r="AW41" s="91"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" s="2"/>
@@ -4780,27 +4729,27 @@
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
       <c r="AD42" s="2"/>
-      <c r="AE42" t="s" s="101">
+      <c r="AE42" t="s" s="92">
         <v>41</v>
       </c>
-      <c r="AF42" s="102"/>
-      <c r="AG42" s="102"/>
-      <c r="AH42" s="102"/>
-      <c r="AI42" s="102"/>
-      <c r="AJ42" s="102"/>
-      <c r="AK42" s="102"/>
-      <c r="AL42" s="102"/>
-      <c r="AM42" s="102"/>
-      <c r="AN42" s="102"/>
-      <c r="AO42" s="102"/>
-      <c r="AP42" s="102"/>
-      <c r="AQ42" s="102"/>
-      <c r="AR42" s="102"/>
-      <c r="AS42" s="102"/>
-      <c r="AT42" s="102"/>
-      <c r="AU42" s="102"/>
-      <c r="AV42" s="102"/>
-      <c r="AW42" s="102"/>
+      <c r="AF42" s="93"/>
+      <c r="AG42" s="93"/>
+      <c r="AH42" s="93"/>
+      <c r="AI42" s="93"/>
+      <c r="AJ42" s="93"/>
+      <c r="AK42" s="93"/>
+      <c r="AL42" s="93"/>
+      <c r="AM42" s="93"/>
+      <c r="AN42" s="93"/>
+      <c r="AO42" s="93"/>
+      <c r="AP42" s="93"/>
+      <c r="AQ42" s="93"/>
+      <c r="AR42" s="93"/>
+      <c r="AS42" s="93"/>
+      <c r="AT42" s="93"/>
+      <c r="AU42" s="93"/>
+      <c r="AV42" s="93"/>
+      <c r="AW42" s="93"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2"/>
@@ -4833,25 +4782,25 @@
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
       <c r="AD43" s="2"/>
-      <c r="AE43" s="99"/>
-      <c r="AF43" s="99"/>
-      <c r="AG43" s="99"/>
-      <c r="AH43" s="99"/>
-      <c r="AI43" s="99"/>
-      <c r="AJ43" s="99"/>
-      <c r="AK43" s="99"/>
-      <c r="AL43" s="99"/>
-      <c r="AM43" s="99"/>
-      <c r="AN43" s="99"/>
-      <c r="AO43" s="99"/>
-      <c r="AP43" s="99"/>
-      <c r="AQ43" s="99"/>
-      <c r="AR43" s="99"/>
-      <c r="AS43" s="99"/>
-      <c r="AT43" s="99"/>
-      <c r="AU43" s="99"/>
-      <c r="AV43" s="99"/>
-      <c r="AW43" s="99"/>
+      <c r="AE43" s="90"/>
+      <c r="AF43" s="90"/>
+      <c r="AG43" s="90"/>
+      <c r="AH43" s="90"/>
+      <c r="AI43" s="90"/>
+      <c r="AJ43" s="90"/>
+      <c r="AK43" s="90"/>
+      <c r="AL43" s="90"/>
+      <c r="AM43" s="90"/>
+      <c r="AN43" s="90"/>
+      <c r="AO43" s="90"/>
+      <c r="AP43" s="90"/>
+      <c r="AQ43" s="90"/>
+      <c r="AR43" s="90"/>
+      <c r="AS43" s="90"/>
+      <c r="AT43" s="90"/>
+      <c r="AU43" s="90"/>
+      <c r="AV43" s="90"/>
+      <c r="AW43" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="217">

</xml_diff>